<commit_message>
Update 2022-23 ADS&AI Assessment Rubric Block A.xlsx
</commit_message>
<xml_diff>
--- a/docs/Year1/BlockA/MS Teams Assignment Template/2022-23 ADS&AI Assessment Rubric Block A.xlsx
+++ b/docs/Year1/BlockA/MS Teams Assignment Template/2022-23 ADS&AI Assessment Rubric Block A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramh\Documents\GitHub\AAI-DM\docs\Year1\BlockA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramh\Documents\GitHub\AAI-DM\docs\Year1\BlockA\MS Teams Assignment Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF32CE88-AAFD-4F6E-ABCB-688B87A1C875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BBAA40-F03D-4A30-B8C5-1F117AF9B164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="3495" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Self-Assessment" sheetId="1" r:id="rId1"/>
@@ -1572,38 +1572,62 @@
     <xf numFmtId="0" fontId="24" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1624,40 +1648,16 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1671,10 +1671,10 @@
     <xf numFmtId="0" fontId="19" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2151,8 +2151,8 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19:K19"/>
+      <pane ySplit="10" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2204,11 +2204,11 @@
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="37"/>
       <c r="B2" s="38"/>
-      <c r="C2" s="126" t="s">
+      <c r="C2" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
       <c r="H2" s="38"/>
@@ -2234,8 +2234,8 @@
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="120"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="122"/>
       <c r="E3" s="41" t="s">
         <v>1</v>
       </c>
@@ -2245,15 +2245,15 @@
       <c r="G3" s="42"/>
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
-      <c r="J3" s="131" t="s">
+      <c r="J3" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="120"/>
-      <c r="L3" s="133" t="s">
+      <c r="K3" s="122"/>
+      <c r="L3" s="141" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="120"/>
-      <c r="N3" s="120"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
       <c r="O3" s="40"/>
       <c r="P3" s="39"/>
       <c r="Q3" s="2"/>
@@ -2270,27 +2270,27 @@
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="37"/>
       <c r="B4" s="45"/>
-      <c r="C4" s="142" t="s">
+      <c r="C4" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="120"/>
+      <c r="D4" s="122"/>
       <c r="E4" s="46"/>
-      <c r="F4" s="134" t="s">
+      <c r="F4" s="142" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="135"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="140" t="s">
+      <c r="G4" s="122"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="141">
+      <c r="M4" s="137">
         <f>IF(ROUND((N22/10),1)&lt;&gt;ROUND((N22/10),0),ROUND((N22/10),1),ROUND((N22/10),0))</f>
         <v>0</v>
       </c>
-      <c r="N4" s="136" t="str">
+      <c r="N4" s="144" t="str">
         <f>IF(M4&gt;=5.5,"PASS",IF(M4&gt;0,"FAIL","M/O"))</f>
         <v>M/O</v>
       </c>
@@ -2310,20 +2310,20 @@
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="37"/>
       <c r="B5" s="45"/>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="120"/>
+      <c r="D5" s="122"/>
       <c r="E5" s="46"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="128"/>
-      <c r="N5" s="128"/>
+      <c r="F5" s="122"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="122"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="134"/>
       <c r="O5" s="38"/>
       <c r="P5" s="37"/>
       <c r="Q5" s="1"/>
@@ -2340,22 +2340,22 @@
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="37"/>
       <c r="B6" s="45"/>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="120"/>
+      <c r="D6" s="122"/>
       <c r="E6" s="47" t="s">
         <v>195</v>
       </c>
-      <c r="F6" s="120"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="128"/>
-      <c r="N6" s="128"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
       <c r="O6" s="38"/>
       <c r="P6" s="37"/>
       <c r="Q6" s="1"/>
@@ -2372,22 +2372,22 @@
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="37"/>
       <c r="B7" s="45"/>
-      <c r="C7" s="142" t="s">
+      <c r="C7" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="120"/>
+      <c r="D7" s="122"/>
       <c r="E7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="120"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="128"/>
-      <c r="N7" s="128"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="122"/>
+      <c r="M7" s="134"/>
+      <c r="N7" s="134"/>
       <c r="O7" s="38"/>
       <c r="P7" s="37"/>
       <c r="Q7" s="1"/>
@@ -2404,22 +2404,22 @@
     <row r="8" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="37"/>
       <c r="B8" s="45"/>
-      <c r="C8" s="137" t="s">
+      <c r="C8" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="120"/>
+      <c r="D8" s="122"/>
       <c r="E8" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="F8" s="120"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="128"/>
-      <c r="N8" s="128"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="122"/>
+      <c r="K8" s="122"/>
+      <c r="L8" s="122"/>
+      <c r="M8" s="134"/>
+      <c r="N8" s="134"/>
       <c r="O8" s="38"/>
       <c r="P8" s="37"/>
       <c r="Q8" s="1"/>
@@ -2492,11 +2492,11 @@
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="37"/>
       <c r="B11" s="38"/>
-      <c r="C11" s="126" t="s">
+      <c r="C11" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
@@ -2570,19 +2570,19 @@
     <row r="13" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
       <c r="B13" s="38"/>
-      <c r="C13" s="138" t="s">
+      <c r="C13" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="144" t="s">
+      <c r="D13" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="122"/>
       <c r="L13" s="54"/>
       <c r="M13" s="54"/>
       <c r="N13" s="54"/>
@@ -2602,11 +2602,11 @@
     <row r="14" spans="1:26" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="37"/>
       <c r="B14" s="38"/>
-      <c r="C14" s="128"/>
-      <c r="D14" s="145" t="s">
+      <c r="C14" s="134"/>
+      <c r="D14" s="119" t="s">
         <v>194</v>
       </c>
-      <c r="E14" s="146"/>
+      <c r="E14" s="120"/>
       <c r="F14" s="56" t="s">
         <v>191</v>
       </c>
@@ -2651,19 +2651,19 @@
     <row r="15" spans="1:26" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37"/>
       <c r="B15" s="38"/>
-      <c r="C15" s="138" t="s">
+      <c r="C15" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="143" t="s">
+      <c r="D15" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="122"/>
+      <c r="G15" s="122"/>
+      <c r="H15" s="122"/>
+      <c r="I15" s="122"/>
+      <c r="J15" s="122"/>
+      <c r="K15" s="122"/>
       <c r="L15" s="64"/>
       <c r="M15" s="64"/>
       <c r="N15" s="64"/>
@@ -2683,11 +2683,11 @@
     <row r="16" spans="1:26" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="128"/>
-      <c r="D16" s="139" t="s">
+      <c r="C16" s="134"/>
+      <c r="D16" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="128"/>
+      <c r="E16" s="134"/>
       <c r="F16" s="56" t="s">
         <v>191</v>
       </c>
@@ -2732,19 +2732,19 @@
     <row r="17" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="38"/>
-      <c r="C17" s="138" t="s">
+      <c r="C17" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="148" t="s">
+      <c r="D17" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="120"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="122"/>
+      <c r="H17" s="122"/>
+      <c r="I17" s="122"/>
+      <c r="J17" s="122"/>
+      <c r="K17" s="122"/>
       <c r="L17" s="65"/>
       <c r="M17" s="65"/>
       <c r="N17" s="65"/>
@@ -2764,11 +2764,11 @@
     <row r="18" spans="1:26" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="38"/>
-      <c r="C18" s="128"/>
-      <c r="D18" s="139" t="s">
+      <c r="C18" s="134"/>
+      <c r="D18" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="128"/>
+      <c r="E18" s="134"/>
       <c r="F18" s="66" t="s">
         <v>192</v>
       </c>
@@ -2813,19 +2813,19 @@
     <row r="19" spans="1:26" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="138" t="s">
+      <c r="C19" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="144" t="s">
+      <c r="D19" s="126" t="s">
         <v>203</v>
       </c>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="120"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="120"/>
-      <c r="J19" s="120"/>
-      <c r="K19" s="120"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="122"/>
+      <c r="H19" s="122"/>
+      <c r="I19" s="122"/>
+      <c r="J19" s="122"/>
+      <c r="K19" s="122"/>
       <c r="L19" s="54"/>
       <c r="M19" s="54"/>
       <c r="N19" s="54"/>
@@ -2845,11 +2845,11 @@
     <row r="20" spans="1:26" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="67"/>
       <c r="B20" s="68"/>
-      <c r="C20" s="128"/>
-      <c r="D20" s="139" t="s">
+      <c r="C20" s="134"/>
+      <c r="D20" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="128"/>
+      <c r="E20" s="134"/>
       <c r="F20" s="56" t="s">
         <v>191</v>
       </c>
@@ -2894,11 +2894,11 @@
     <row r="21" spans="1:26" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="72"/>
       <c r="B21" s="73"/>
-      <c r="C21" s="128"/>
-      <c r="D21" s="147" t="s">
+      <c r="C21" s="134"/>
+      <c r="D21" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="120"/>
+      <c r="E21" s="122"/>
       <c r="F21" s="56" t="s">
         <v>191</v>
       </c>
@@ -2949,11 +2949,11 @@
       <c r="F22" s="38"/>
       <c r="G22" s="38"/>
       <c r="H22" s="38"/>
-      <c r="I22" s="149" t="s">
+      <c r="I22" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="120"/>
-      <c r="K22" s="120"/>
+      <c r="J22" s="122"/>
+      <c r="K22" s="122"/>
       <c r="L22" s="77">
         <f>SUM(L14:L21)</f>
         <v>100</v>
@@ -2962,7 +2962,7 @@
         <v>48</v>
       </c>
       <c r="N22" s="62">
-        <f>SUM(N16:N21)</f>
+        <f>SUM(N14:N21)</f>
         <v>0</v>
       </c>
       <c r="O22" s="55"/>
@@ -3037,11 +3037,11 @@
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="37"/>
       <c r="B25" s="79"/>
-      <c r="C25" s="126" t="s">
+      <c r="C25" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
       <c r="F25" s="79"/>
       <c r="G25" s="79"/>
       <c r="H25" s="79"/>
@@ -3070,20 +3070,20 @@
       <c r="C26" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="131" t="s">
+      <c r="D26" s="132" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="120"/>
+      <c r="E26" s="122"/>
       <c r="F26" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="131" t="s">
+      <c r="G26" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="H26" s="120"/>
-      <c r="I26" s="120"/>
-      <c r="J26" s="120"/>
-      <c r="K26" s="120"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="122"/>
+      <c r="K26" s="122"/>
       <c r="L26" s="81"/>
       <c r="M26" s="44"/>
       <c r="N26" s="48" t="s">
@@ -3108,22 +3108,22 @@
       <c r="C27" s="82">
         <v>9</v>
       </c>
-      <c r="D27" s="121" t="s">
+      <c r="D27" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="120"/>
+      <c r="E27" s="122"/>
       <c r="F27" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="119" t="s">
+      <c r="G27" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="H27" s="120"/>
-      <c r="I27" s="120"/>
-      <c r="J27" s="120"/>
-      <c r="K27" s="120"/>
-      <c r="L27" s="120"/>
-      <c r="M27" s="120"/>
+      <c r="H27" s="122"/>
+      <c r="I27" s="122"/>
+      <c r="J27" s="122"/>
+      <c r="K27" s="122"/>
+      <c r="L27" s="122"/>
+      <c r="M27" s="122"/>
       <c r="N27" s="84">
         <v>3</v>
       </c>
@@ -3146,22 +3146,22 @@
       <c r="C28" s="82">
         <v>10</v>
       </c>
-      <c r="D28" s="121" t="s">
+      <c r="D28" s="149" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="120"/>
+      <c r="E28" s="122"/>
       <c r="F28" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="G28" s="119" t="s">
+      <c r="G28" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="H28" s="120"/>
-      <c r="I28" s="120"/>
-      <c r="J28" s="120"/>
-      <c r="K28" s="120"/>
-      <c r="L28" s="120"/>
-      <c r="M28" s="120"/>
+      <c r="H28" s="122"/>
+      <c r="I28" s="122"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="122"/>
+      <c r="L28" s="122"/>
+      <c r="M28" s="122"/>
       <c r="N28" s="84">
         <v>3</v>
       </c>
@@ -3184,22 +3184,22 @@
       <c r="C29" s="82">
         <v>11</v>
       </c>
-      <c r="D29" s="121" t="s">
+      <c r="D29" s="149" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="120"/>
+      <c r="E29" s="122"/>
       <c r="F29" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="119" t="s">
+      <c r="G29" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="H29" s="120"/>
-      <c r="I29" s="120"/>
-      <c r="J29" s="120"/>
-      <c r="K29" s="120"/>
-      <c r="L29" s="120"/>
-      <c r="M29" s="120"/>
+      <c r="H29" s="122"/>
+      <c r="I29" s="122"/>
+      <c r="J29" s="122"/>
+      <c r="K29" s="122"/>
+      <c r="L29" s="122"/>
+      <c r="M29" s="122"/>
       <c r="N29" s="84">
         <v>3</v>
       </c>
@@ -3222,22 +3222,22 @@
       <c r="C30" s="85">
         <v>1</v>
       </c>
-      <c r="D30" s="122" t="s">
+      <c r="D30" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="120"/>
+      <c r="E30" s="122"/>
       <c r="F30" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="123" t="s">
+      <c r="G30" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="H30" s="120"/>
-      <c r="I30" s="120"/>
-      <c r="J30" s="120"/>
-      <c r="K30" s="120"/>
-      <c r="L30" s="120"/>
-      <c r="M30" s="120"/>
+      <c r="H30" s="122"/>
+      <c r="I30" s="122"/>
+      <c r="J30" s="122"/>
+      <c r="K30" s="122"/>
+      <c r="L30" s="122"/>
+      <c r="M30" s="122"/>
       <c r="N30" s="87">
         <v>3</v>
       </c>
@@ -3260,22 +3260,22 @@
       <c r="C31" s="88">
         <v>2</v>
       </c>
-      <c r="D31" s="124" t="s">
+      <c r="D31" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="120"/>
+      <c r="E31" s="122"/>
       <c r="F31" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="125" t="s">
+      <c r="G31" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="120"/>
-      <c r="I31" s="120"/>
-      <c r="J31" s="120"/>
-      <c r="K31" s="120"/>
-      <c r="L31" s="120"/>
-      <c r="M31" s="120"/>
+      <c r="H31" s="122"/>
+      <c r="I31" s="122"/>
+      <c r="J31" s="122"/>
+      <c r="K31" s="122"/>
+      <c r="L31" s="122"/>
+      <c r="M31" s="122"/>
       <c r="N31" s="90">
         <v>3</v>
       </c>
@@ -3298,22 +3298,22 @@
       <c r="C32" s="85">
         <v>3</v>
       </c>
-      <c r="D32" s="122" t="s">
+      <c r="D32" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="120"/>
+      <c r="E32" s="122"/>
       <c r="F32" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="123" t="s">
+      <c r="G32" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="H32" s="120"/>
-      <c r="I32" s="120"/>
-      <c r="J32" s="120"/>
-      <c r="K32" s="120"/>
-      <c r="L32" s="120"/>
-      <c r="M32" s="120"/>
+      <c r="H32" s="122"/>
+      <c r="I32" s="122"/>
+      <c r="J32" s="122"/>
+      <c r="K32" s="122"/>
+      <c r="L32" s="122"/>
+      <c r="M32" s="122"/>
       <c r="N32" s="87">
         <v>3</v>
       </c>
@@ -3336,22 +3336,22 @@
       <c r="C33" s="88">
         <v>4</v>
       </c>
-      <c r="D33" s="124" t="s">
+      <c r="D33" s="123" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="120"/>
+      <c r="E33" s="122"/>
       <c r="F33" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="125" t="s">
+      <c r="G33" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="H33" s="120"/>
-      <c r="I33" s="120"/>
-      <c r="J33" s="120"/>
-      <c r="K33" s="120"/>
-      <c r="L33" s="120"/>
-      <c r="M33" s="120"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="122"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="122"/>
+      <c r="L33" s="122"/>
+      <c r="M33" s="122"/>
       <c r="N33" s="90">
         <v>3</v>
       </c>
@@ -3374,22 +3374,22 @@
       <c r="C34" s="91">
         <v>5</v>
       </c>
-      <c r="D34" s="122" t="s">
+      <c r="D34" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="120"/>
+      <c r="E34" s="122"/>
       <c r="F34" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="G34" s="123" t="s">
+      <c r="G34" s="129" t="s">
         <v>74</v>
       </c>
-      <c r="H34" s="120"/>
-      <c r="I34" s="120"/>
-      <c r="J34" s="120"/>
-      <c r="K34" s="120"/>
-      <c r="L34" s="120"/>
-      <c r="M34" s="120"/>
+      <c r="H34" s="122"/>
+      <c r="I34" s="122"/>
+      <c r="J34" s="122"/>
+      <c r="K34" s="122"/>
+      <c r="L34" s="122"/>
+      <c r="M34" s="122"/>
       <c r="N34" s="87">
         <v>3</v>
       </c>
@@ -3412,22 +3412,22 @@
       <c r="C35" s="88">
         <v>6</v>
       </c>
-      <c r="D35" s="124" t="s">
+      <c r="D35" s="123" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="120"/>
+      <c r="E35" s="122"/>
       <c r="F35" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="G35" s="125" t="s">
+      <c r="G35" s="128" t="s">
         <v>76</v>
       </c>
-      <c r="H35" s="120"/>
-      <c r="I35" s="120"/>
-      <c r="J35" s="120"/>
-      <c r="K35" s="120"/>
-      <c r="L35" s="120"/>
-      <c r="M35" s="120"/>
+      <c r="H35" s="122"/>
+      <c r="I35" s="122"/>
+      <c r="J35" s="122"/>
+      <c r="K35" s="122"/>
+      <c r="L35" s="122"/>
+      <c r="M35" s="122"/>
       <c r="N35" s="90">
         <v>3</v>
       </c>
@@ -3450,22 +3450,22 @@
       <c r="C36" s="85">
         <v>7</v>
       </c>
-      <c r="D36" s="122" t="s">
+      <c r="D36" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="120"/>
+      <c r="E36" s="122"/>
       <c r="F36" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="123" t="s">
+      <c r="G36" s="129" t="s">
         <v>79</v>
       </c>
-      <c r="H36" s="120"/>
-      <c r="I36" s="120"/>
-      <c r="J36" s="120"/>
-      <c r="K36" s="120"/>
-      <c r="L36" s="120"/>
-      <c r="M36" s="120"/>
+      <c r="H36" s="122"/>
+      <c r="I36" s="122"/>
+      <c r="J36" s="122"/>
+      <c r="K36" s="122"/>
+      <c r="L36" s="122"/>
+      <c r="M36" s="122"/>
       <c r="N36" s="87">
         <v>3</v>
       </c>
@@ -3488,22 +3488,22 @@
       <c r="C37" s="88">
         <v>8</v>
       </c>
-      <c r="D37" s="124" t="s">
+      <c r="D37" s="123" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="120"/>
+      <c r="E37" s="122"/>
       <c r="F37" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="G37" s="125" t="s">
+      <c r="G37" s="128" t="s">
         <v>81</v>
       </c>
-      <c r="H37" s="120"/>
-      <c r="I37" s="120"/>
-      <c r="J37" s="120"/>
-      <c r="K37" s="120"/>
-      <c r="L37" s="120"/>
-      <c r="M37" s="120"/>
+      <c r="H37" s="122"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="122"/>
+      <c r="K37" s="122"/>
+      <c r="L37" s="122"/>
+      <c r="M37" s="122"/>
       <c r="N37" s="90">
         <v>3</v>
       </c>
@@ -3579,11 +3579,11 @@
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="37"/>
       <c r="B40" s="92"/>
-      <c r="C40" s="126" t="s">
+      <c r="C40" s="131" t="s">
         <v>82</v>
       </c>
-      <c r="D40" s="120"/>
-      <c r="E40" s="120"/>
+      <c r="D40" s="122"/>
+      <c r="E40" s="122"/>
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
       <c r="H40" s="38"/>
@@ -3616,19 +3616,19 @@
         <v>83</v>
       </c>
       <c r="E41" s="94"/>
-      <c r="F41" s="130" t="s">
+      <c r="F41" s="148" t="s">
         <v>84</v>
       </c>
-      <c r="G41" s="120"/>
-      <c r="H41" s="120"/>
-      <c r="I41" s="120"/>
-      <c r="J41" s="131" t="s">
+      <c r="G41" s="122"/>
+      <c r="H41" s="122"/>
+      <c r="I41" s="122"/>
+      <c r="J41" s="132" t="s">
         <v>85</v>
       </c>
-      <c r="K41" s="120"/>
-      <c r="L41" s="120"/>
-      <c r="M41" s="120"/>
-      <c r="N41" s="120"/>
+      <c r="K41" s="122"/>
+      <c r="L41" s="122"/>
+      <c r="M41" s="122"/>
+      <c r="N41" s="122"/>
       <c r="O41" s="38"/>
       <c r="P41" s="37"/>
       <c r="Q41" s="1"/>
@@ -3652,19 +3652,19 @@
         <v>86</v>
       </c>
       <c r="E42" s="6"/>
-      <c r="F42" s="127" t="s">
+      <c r="F42" s="146" t="s">
         <v>87</v>
       </c>
-      <c r="G42" s="128"/>
-      <c r="H42" s="128"/>
-      <c r="I42" s="128"/>
-      <c r="J42" s="127" t="s">
+      <c r="G42" s="134"/>
+      <c r="H42" s="134"/>
+      <c r="I42" s="134"/>
+      <c r="J42" s="146" t="s">
         <v>88</v>
       </c>
-      <c r="K42" s="128"/>
-      <c r="L42" s="128"/>
-      <c r="M42" s="128"/>
-      <c r="N42" s="128"/>
+      <c r="K42" s="134"/>
+      <c r="L42" s="134"/>
+      <c r="M42" s="134"/>
+      <c r="N42" s="134"/>
       <c r="O42" s="38"/>
       <c r="P42" s="37"/>
       <c r="Q42" s="1"/>
@@ -3688,19 +3688,19 @@
         <v>89</v>
       </c>
       <c r="E43" s="97"/>
-      <c r="F43" s="129" t="s">
+      <c r="F43" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="G43" s="120"/>
-      <c r="H43" s="120"/>
-      <c r="I43" s="120"/>
-      <c r="J43" s="129" t="s">
+      <c r="G43" s="122"/>
+      <c r="H43" s="122"/>
+      <c r="I43" s="122"/>
+      <c r="J43" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="K43" s="120"/>
-      <c r="L43" s="120"/>
-      <c r="M43" s="120"/>
-      <c r="N43" s="120"/>
+      <c r="K43" s="122"/>
+      <c r="L43" s="122"/>
+      <c r="M43" s="122"/>
+      <c r="N43" s="122"/>
       <c r="O43" s="38"/>
       <c r="P43" s="37"/>
       <c r="Q43" s="1"/>
@@ -3724,19 +3724,19 @@
         <v>92</v>
       </c>
       <c r="E44" s="6"/>
-      <c r="F44" s="127" t="s">
+      <c r="F44" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="128"/>
-      <c r="H44" s="128"/>
-      <c r="I44" s="128"/>
-      <c r="J44" s="127" t="s">
+      <c r="G44" s="134"/>
+      <c r="H44" s="134"/>
+      <c r="I44" s="134"/>
+      <c r="J44" s="146" t="s">
         <v>94</v>
       </c>
-      <c r="K44" s="128"/>
-      <c r="L44" s="128"/>
-      <c r="M44" s="128"/>
-      <c r="N44" s="128"/>
+      <c r="K44" s="134"/>
+      <c r="L44" s="134"/>
+      <c r="M44" s="134"/>
+      <c r="N44" s="134"/>
       <c r="O44" s="38"/>
       <c r="P44" s="37"/>
       <c r="Q44" s="1"/>
@@ -3760,19 +3760,19 @@
         <v>95</v>
       </c>
       <c r="E45" s="97"/>
-      <c r="F45" s="129" t="s">
+      <c r="F45" s="147" t="s">
         <v>96</v>
       </c>
-      <c r="G45" s="120"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="120"/>
-      <c r="J45" s="129" t="s">
+      <c r="G45" s="122"/>
+      <c r="H45" s="122"/>
+      <c r="I45" s="122"/>
+      <c r="J45" s="147" t="s">
         <v>97</v>
       </c>
-      <c r="K45" s="120"/>
-      <c r="L45" s="120"/>
-      <c r="M45" s="120"/>
-      <c r="N45" s="120"/>
+      <c r="K45" s="122"/>
+      <c r="L45" s="122"/>
+      <c r="M45" s="122"/>
+      <c r="N45" s="122"/>
       <c r="O45" s="38"/>
       <c r="P45" s="37"/>
       <c r="Q45" s="1"/>
@@ -3796,19 +3796,19 @@
         <v>98</v>
       </c>
       <c r="E46" s="6"/>
-      <c r="F46" s="127" t="s">
+      <c r="F46" s="146" t="s">
         <v>99</v>
       </c>
-      <c r="G46" s="128"/>
-      <c r="H46" s="128"/>
-      <c r="I46" s="128"/>
-      <c r="J46" s="127" t="s">
+      <c r="G46" s="134"/>
+      <c r="H46" s="134"/>
+      <c r="I46" s="134"/>
+      <c r="J46" s="146" t="s">
         <v>100</v>
       </c>
-      <c r="K46" s="128"/>
-      <c r="L46" s="128"/>
-      <c r="M46" s="128"/>
-      <c r="N46" s="128"/>
+      <c r="K46" s="134"/>
+      <c r="L46" s="134"/>
+      <c r="M46" s="134"/>
+      <c r="N46" s="134"/>
       <c r="O46" s="38"/>
       <c r="P46" s="37"/>
       <c r="Q46" s="1"/>
@@ -30536,6 +30536,57 @@
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="G27:M27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:M36"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G30:M30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:M31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="G32:M32"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G37:M37"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="J45:N45"/>
+    <mergeCell ref="J46:N46"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="J41:N41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="J42:N42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="J44:N44"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="F4:I8"/>
+    <mergeCell ref="J4:K8"/>
+    <mergeCell ref="N4:N8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="L4:L8"/>
+    <mergeCell ref="M4:M8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:K13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D33:E33"/>
@@ -30552,57 +30603,6 @@
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="G26:K26"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="L4:L8"/>
-    <mergeCell ref="M4:M8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:K13"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="F4:I8"/>
-    <mergeCell ref="J4:K8"/>
-    <mergeCell ref="N4:N8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="J45:N45"/>
-    <mergeCell ref="J46:N46"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="J41:N41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="J42:N42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="J44:N44"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G37:M37"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="G27:M27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:M36"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G30:M30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:M31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="G32:M32"/>
-    <mergeCell ref="D27:E27"/>
   </mergeCells>
   <conditionalFormatting sqref="N4">
     <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="FAIL">
@@ -30781,8 +30781,8 @@
       <c r="B2" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
       <c r="G2" s="8"/>
       <c r="H2" s="98" t="s">
         <v>103</v>
@@ -30847,8 +30847,8 @@
       <c r="B5" s="150" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
       <c r="F5" s="7">
         <v>6.1</v>
       </c>
@@ -30934,8 +30934,8 @@
       <c r="B7" s="150" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="120"/>
-      <c r="D7" s="120"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
       <c r="F7" s="7">
         <v>6.2</v>
       </c>
@@ -30990,8 +30990,8 @@
       <c r="B8" s="150" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
       <c r="G8" s="8"/>
       <c r="H8" s="105" t="s">
         <v>117</v>
@@ -31056,8 +31056,8 @@
     </row>
     <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="151"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
       <c r="G13" s="7"/>
       <c r="H13" s="8" t="s">
         <v>137</v>
@@ -31082,8 +31082,8 @@
       <c r="B14" s="150" t="s">
         <v>143</v>
       </c>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
       <c r="F14" s="7">
         <v>3.1</v>
       </c>
@@ -31177,8 +31177,8 @@
       <c r="B18" s="150" t="s">
         <v>155</v>
       </c>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
       <c r="F18" s="7">
         <v>3.2</v>
       </c>
@@ -31293,8 +31293,8 @@
       <c r="B25" s="151" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
+      <c r="C25" s="122"/>
+      <c r="D25" s="122"/>
       <c r="G25" s="7" t="s">
         <v>168</v>
       </c>
@@ -32366,12 +32366,12 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="156"/>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
       <c r="H2" s="157"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -32396,25 +32396,25 @@
       <c r="A3" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="120"/>
+      <c r="B3" s="122"/>
       <c r="C3" s="109" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="159" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
       <c r="H3" s="157"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="160" t="s">
         <v>177</v>
       </c>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="120"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
       <c r="O3" s="110"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
@@ -60462,6 +60462,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064DEF28CA2629948A9F801C782641252" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5d88cf87ad5ac9fc8fb83d77fe1635d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bd38d267-56bb-4e22-b975-199a06fd69fa" xmlns:ns3="d8c712e5-67fc-4595-93cb-a4164dd8eff3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d44111b7d9e9f445610cec830697d19" ns2:_="" ns3:_="">
     <xsd:import namespace="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
@@ -60676,12 +60682,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D1E7A10-6C2D-4580-A4D2-EC7B8465FD38}">
   <ds:schemaRefs>
@@ -60691,6 +60691,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5072705-B970-4C6A-9B95-6E8AEA4192EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A82C80A-75CE-43A3-BF6C-CAF5684B7966}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -60707,21 +60724,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5072705-B970-4C6A-9B95-6E8AEA4192EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>